<commit_message>
Capstone Project Data Story
Capstone Project Data Story
</commit_message>
<xml_diff>
--- a/datacig.xlsx
+++ b/datacig.xlsx
@@ -1,27 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TC/Desktop/tum dosyalar/The Effect of Regulation and Taxation on Smoking/sigara data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TC/Desktop/Springboard Data Science Bootcamp/data_wrangling_json/Capstone-Project-1--Data-Story/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60C021F-3E79-994A-A13F-199E85EBE2DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="monthly" sheetId="1" r:id="rId1"/>
-    <sheet name="quarterly" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -62,149 +67,11 @@
   <si>
     <t>D5jan13mixstrtgy</t>
   </si>
-  <si>
-    <t>lngdp</t>
-  </si>
-  <si>
-    <t>Dregjuly09</t>
-  </si>
-  <si>
-    <t>Dtaxjan10</t>
-  </si>
-  <si>
-    <t>Dtaxoct11</t>
-  </si>
-  <si>
-    <t>Djul12reg(total advertisement ban)</t>
-  </si>
-  <si>
-    <t>Djan13mixstrtgy</t>
-  </si>
-  <si>
-    <t>2005q1</t>
-  </si>
-  <si>
-    <t>2005q2</t>
-  </si>
-  <si>
-    <t>2005q3</t>
-  </si>
-  <si>
-    <t>2005q4</t>
-  </si>
-  <si>
-    <t>2006q1</t>
-  </si>
-  <si>
-    <t>2006q2</t>
-  </si>
-  <si>
-    <t>2006q3</t>
-  </si>
-  <si>
-    <t>2006q4</t>
-  </si>
-  <si>
-    <t>2007q1</t>
-  </si>
-  <si>
-    <t>2007q2</t>
-  </si>
-  <si>
-    <t>2007q3</t>
-  </si>
-  <si>
-    <t>2007q4</t>
-  </si>
-  <si>
-    <t>2008q1</t>
-  </si>
-  <si>
-    <t>2008q2</t>
-  </si>
-  <si>
-    <t>2008q3</t>
-  </si>
-  <si>
-    <t>2008q4</t>
-  </si>
-  <si>
-    <t>2009q1</t>
-  </si>
-  <si>
-    <t>2009q2</t>
-  </si>
-  <si>
-    <t>2009q3</t>
-  </si>
-  <si>
-    <t>2009q4</t>
-  </si>
-  <si>
-    <t>2010q1</t>
-  </si>
-  <si>
-    <t>2010q2</t>
-  </si>
-  <si>
-    <t>2010q3</t>
-  </si>
-  <si>
-    <t>2010q4</t>
-  </si>
-  <si>
-    <t>2011q1</t>
-  </si>
-  <si>
-    <t>2011q2</t>
-  </si>
-  <si>
-    <t>2011q3</t>
-  </si>
-  <si>
-    <t>2011q4</t>
-  </si>
-  <si>
-    <t>2012q1</t>
-  </si>
-  <si>
-    <t>2012q2</t>
-  </si>
-  <si>
-    <t>2012q3</t>
-  </si>
-  <si>
-    <t>2012q4</t>
-  </si>
-  <si>
-    <t>2013q1</t>
-  </si>
-  <si>
-    <t>2013q2</t>
-  </si>
-  <si>
-    <t>2013q3</t>
-  </si>
-  <si>
-    <t>2013q4</t>
-  </si>
-  <si>
-    <t>2014q1</t>
-  </si>
-  <si>
-    <t>2014q2</t>
-  </si>
-  <si>
-    <t>2014q3</t>
-  </si>
-  <si>
-    <t>2014q4</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -281,11 +148,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -314,224 +180,11 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="H2">
-            <v>19947283</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="H3">
-            <v>21577563</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="H4">
-            <v>25323570</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="H5">
-            <v>23651315</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="H6">
-            <v>21133291</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="H7">
-            <v>23678188</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="H8">
-            <v>26916390</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="H9">
-            <v>25010451</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="H10">
-            <v>22844200</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="H11">
-            <v>24581028</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="H12">
-            <v>27772167</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="H13">
-            <v>26057230</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="H14">
-            <v>24445513</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="H15">
-            <v>25226375</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="H16">
-            <v>28009692</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="H17">
-            <v>24240150</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="H18">
-            <v>20842792</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="H19">
-            <v>23267231</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="H20">
-            <v>27233060</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="H21">
-            <v>25660031</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="H22">
-            <v>23467330</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="H23">
-            <v>25692252</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="H24">
-            <v>28669613</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="H25">
-            <v>28056450</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="H26">
-            <v>26382817</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="H27">
-            <v>28082510</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="H28">
-            <v>31176687</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="H29">
-            <v>29532710</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="H30">
-            <v>27196829</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="H31">
-            <v>28854662</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="H32">
-            <v>31643556</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="H33">
-            <v>29929974</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="H34">
-            <v>28047894</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="H35">
-            <v>30204750</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="H36">
-            <v>33005549</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="H37">
-            <v>31298268</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="H38">
-            <v>29412757</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="H39">
-            <v>30907420</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="H40">
-            <v>33645425</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="H41">
-            <v>32104188</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -855,12 +508,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -909,7 +560,7 @@
       <c r="D2">
         <v>-4.6051701859880909</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>4.4414740933173018</v>
       </c>
       <c r="F2">
@@ -941,7 +592,7 @@
       <c r="D3">
         <v>-4.6051701859880909</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>4.2986450257348308</v>
       </c>
       <c r="F3">
@@ -973,7 +624,7 @@
       <c r="D4">
         <v>-4.6051701859880909</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>4.4176350621412492</v>
       </c>
       <c r="F4">
@@ -1005,7 +656,7 @@
       <c r="D5">
         <v>-4.6051701859880909</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>4.3515674271891731</v>
       </c>
       <c r="F5">
@@ -1037,7 +688,7 @@
       <c r="D6">
         <v>-4.6051701859880909</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>4.4188406077965983</v>
       </c>
       <c r="F6">
@@ -1069,7 +720,7 @@
       <c r="D7">
         <v>-4.6051701859880909</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>4.4942386252808095</v>
       </c>
       <c r="F7">
@@ -1101,7 +752,7 @@
       <c r="D8">
         <v>-4.6051701859880909</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>4.4379342666121779</v>
       </c>
       <c r="F8">
@@ -1133,7 +784,7 @@
       <c r="D9">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>4.42484663185681</v>
       </c>
       <c r="F9">
@@ -1165,7 +816,7 @@
       <c r="D10">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>4.5859873665713176</v>
       </c>
       <c r="F10">
@@ -1197,7 +848,7 @@
       <c r="D11">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>4.7122292582814991</v>
       </c>
       <c r="F11">
@@ -1229,7 +880,7 @@
       <c r="D12">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>4.6830567246451622</v>
       </c>
       <c r="F12">
@@ -1261,7 +912,7 @@
       <c r="D13">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>4.6700211583077076</v>
       </c>
       <c r="F13">
@@ -1293,7 +944,7 @@
       <c r="D14">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>4.4284330074880369</v>
       </c>
       <c r="F14">
@@ -1325,7 +976,7 @@
       <c r="D15">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>4.4067192472642533</v>
       </c>
       <c r="F15">
@@ -1357,7 +1008,7 @@
       <c r="D16">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>4.5347477216915459</v>
       </c>
       <c r="F16">
@@ -1389,7 +1040,7 @@
       <c r="D17">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>4.4402955427978572</v>
       </c>
       <c r="F17">
@@ -1421,7 +1072,7 @@
       <c r="D18">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>4.4931206821794687</v>
       </c>
       <c r="F18">
@@ -1453,7 +1104,7 @@
       <c r="D19">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>4.5570298106601568</v>
       </c>
       <c r="F19">
@@ -1485,7 +1136,7 @@
       <c r="D20">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>4.4852598893155342</v>
       </c>
       <c r="F20">
@@ -1517,7 +1168,7 @@
       <c r="D21">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>4.4908810395859637</v>
       </c>
       <c r="F21">
@@ -1549,7 +1200,7 @@
       <c r="D22">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>4.5930976047538223</v>
       </c>
       <c r="F22">
@@ -1581,7 +1232,7 @@
       <c r="D23">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>4.6765601820747644</v>
       </c>
       <c r="F23">
@@ -1613,7 +1264,7 @@
       <c r="D24">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="3">
         <v>4.6615505194241988</v>
       </c>
       <c r="F24">
@@ -1645,7 +1296,7 @@
       <c r="D25">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="3">
         <v>4.6587109529161213</v>
       </c>
       <c r="F25">
@@ -1677,7 +1328,7 @@
       <c r="D26">
         <v>-2.8134107167600364</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="3">
         <v>4.5020294270685781</v>
       </c>
       <c r="F26">
@@ -1709,7 +1360,7 @@
       <c r="D27">
         <v>-2.6592600369327779</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="3">
         <v>4.4461744544976334</v>
       </c>
       <c r="F27">
@@ -1741,7 +1392,7 @@
       <c r="D28">
         <v>-2.6592600369327779</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="3">
         <v>4.5705787412184726</v>
       </c>
       <c r="F28">
@@ -1773,7 +1424,7 @@
       <c r="D29">
         <v>-2.6592600369327779</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="3">
         <v>4.514150787600923</v>
       </c>
       <c r="F29">
@@ -1805,7 +1456,7 @@
       <c r="D30">
         <v>-2.6592600369327779</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="3">
         <v>4.577798989191959</v>
       </c>
       <c r="F30">
@@ -1837,7 +1488,7 @@
       <c r="D31">
         <v>-2.6592600369327779</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="3">
         <v>4.5798523780038014</v>
       </c>
       <c r="F31">
@@ -1869,7 +1520,7 @@
       <c r="D32">
         <v>-2.6592600369327779</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="3">
         <v>4.5747109785033828</v>
       </c>
       <c r="F32">
@@ -1901,7 +1552,7 @@
       <c r="D33">
         <v>-2.6592600369327779</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="3">
         <v>4.577798989191959</v>
       </c>
       <c r="F33">
@@ -1933,7 +1584,7 @@
       <c r="D34">
         <v>-2.6592600369327779</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="3">
         <v>4.6395716127054234</v>
       </c>
       <c r="F34">
@@ -1965,7 +1616,7 @@
       <c r="D35">
         <v>-2.6592600369327779</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="3">
         <v>4.7238417157055901</v>
       </c>
       <c r="F35">
@@ -1997,7 +1648,7 @@
       <c r="D36">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="3">
         <v>4.7353208704531369</v>
       </c>
       <c r="F36">
@@ -2029,7 +1680,7 @@
       <c r="D37">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="3">
         <v>4.6746962486367014</v>
       </c>
       <c r="F37">
@@ -2061,7 +1712,7 @@
       <c r="D38">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="3">
         <v>4.4953553199808844</v>
       </c>
       <c r="F38">
@@ -2093,7 +1744,7 @@
       <c r="D39">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="3">
         <v>4.4796069630127455</v>
       </c>
       <c r="F39">
@@ -2125,7 +1776,7 @@
       <c r="D40">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="3">
         <v>4.5400981892443761</v>
       </c>
       <c r="F40">
@@ -2157,7 +1808,7 @@
       <c r="D41">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="3">
         <v>4.4807401076099147</v>
       </c>
       <c r="F41">
@@ -2189,7 +1840,7 @@
       <c r="D42">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="3">
         <v>4.5464811896394117</v>
       </c>
       <c r="F42">
@@ -2221,7 +1872,7 @@
       <c r="D43">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="3">
         <v>4.5767707114663931</v>
       </c>
       <c r="F43">
@@ -2253,7 +1904,7 @@
       <c r="D44">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="3">
         <v>4.5185223792624196</v>
       </c>
       <c r="F44">
@@ -2285,7 +1936,7 @@
       <c r="D45">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="3">
         <v>4.5716134024592483</v>
       </c>
       <c r="F45">
@@ -2317,7 +1968,7 @@
       <c r="D46">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46" s="3">
         <v>4.604169685654508</v>
       </c>
       <c r="F46">
@@ -2349,7 +2000,7 @@
       <c r="D47">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E47" s="4">
+      <c r="E47" s="3">
         <v>4.69866052907543</v>
       </c>
       <c r="F47">
@@ -2381,7 +2032,7 @@
       <c r="D48">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E48" s="4">
+      <c r="E48" s="3">
         <v>4.7414478042806394</v>
       </c>
       <c r="F48">
@@ -2413,7 +2064,7 @@
       <c r="D49">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E49" s="4">
+      <c r="E49" s="3">
         <v>4.6472713620067267</v>
       </c>
       <c r="F49">
@@ -2445,7 +2096,7 @@
       <c r="D50">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E50" s="4">
+      <c r="E50" s="3">
         <v>4.401829261970061</v>
       </c>
       <c r="F50">
@@ -2477,7 +2128,7 @@
       <c r="D51">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E51" s="4">
+      <c r="E51" s="3">
         <v>4.3554259528767023</v>
       </c>
       <c r="F51">
@@ -2509,7 +2160,7 @@
       <c r="D52">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E52" s="4">
+      <c r="E52" s="3">
         <v>4.4659081186545837</v>
       </c>
       <c r="F52">
@@ -2541,7 +2192,7 @@
       <c r="D53">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E53" s="4">
+      <c r="E53" s="3">
         <v>4.4296256134731609</v>
       </c>
       <c r="F53">
@@ -2573,7 +2224,7 @@
       <c r="D54">
         <v>-2.5902671654458267</v>
       </c>
-      <c r="E54" s="4">
+      <c r="E54" s="3">
         <v>4.5086592856072478</v>
       </c>
       <c r="F54">
@@ -2605,7 +2256,7 @@
       <c r="D55">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E55" s="4">
+      <c r="E55" s="3">
         <v>4.5485998344996972</v>
       </c>
       <c r="F55">
@@ -2637,7 +2288,7 @@
       <c r="D56">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E56" s="4">
+      <c r="E56" s="3">
         <v>4.4942386252808095</v>
       </c>
       <c r="F56">
@@ -2669,7 +2320,7 @@
       <c r="D57">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E57" s="4">
+      <c r="E57" s="3">
         <v>4.4807401076099147</v>
       </c>
       <c r="F57">
@@ -2701,7 +2352,7 @@
       <c r="D58">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E58" s="4">
+      <c r="E58" s="3">
         <v>4.5293684725718091</v>
       </c>
       <c r="F58">
@@ -2733,7 +2384,7 @@
       <c r="D59">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E59" s="4">
+      <c r="E59" s="3">
         <v>4.7068238397145912</v>
       </c>
       <c r="F59">
@@ -2765,7 +2416,7 @@
       <c r="D60">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E60" s="7">
+      <c r="E60" s="6">
         <v>4.773223770984341</v>
       </c>
       <c r="F60">
@@ -2797,7 +2448,7 @@
       <c r="D61">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E61" s="7">
+      <c r="E61" s="6">
         <v>4.6885917941271638</v>
       </c>
       <c r="F61">
@@ -2829,7 +2480,7 @@
       <c r="D62">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E62" s="7">
+      <c r="E62" s="6">
         <v>4.4716387933635691</v>
       </c>
       <c r="F62">
@@ -2861,7 +2512,7 @@
       <c r="D63">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E63" s="7">
+      <c r="E63" s="6">
         <v>4.4761998046911318</v>
       </c>
       <c r="F63">
@@ -2893,7 +2544,7 @@
       <c r="D64">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E64" s="7">
+      <c r="E64" s="6">
         <v>4.5685062016164997</v>
       </c>
       <c r="F64">
@@ -2925,7 +2576,7 @@
       <c r="D65">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E65" s="7">
+      <c r="E65" s="6">
         <v>4.5517694092609764</v>
       </c>
       <c r="F65">
@@ -2957,7 +2608,7 @@
       <c r="D66">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E66" s="4">
+      <c r="E66" s="3">
         <v>4.6111522576656387</v>
       </c>
       <c r="F66">
@@ -2989,7 +2640,7 @@
       <c r="D67">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E67" s="4">
+      <c r="E67" s="3">
         <v>4.5971380142908274</v>
       </c>
       <c r="F67">
@@ -3021,7 +2672,7 @@
       <c r="D68">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E68" s="4">
+      <c r="E68" s="3">
         <v>4.5788262106484892</v>
       </c>
       <c r="F68">
@@ -3053,7 +2704,7 @@
       <c r="D69">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E69" s="7">
+      <c r="E69" s="6">
         <v>4.598145571051127</v>
       </c>
       <c r="F69">
@@ -3085,7 +2736,7 @@
       <c r="D70">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E70" s="4">
+      <c r="E70" s="3">
         <v>4.6161101260264257</v>
       </c>
       <c r="F70">
@@ -3117,7 +2768,7 @@
       <c r="D71">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E71" s="4">
+      <c r="E71" s="3">
         <v>4.7431914838854663</v>
       </c>
       <c r="F71">
@@ -3149,7 +2800,7 @@
       <c r="D72">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E72" s="7">
+      <c r="E72" s="6">
         <v>4.7397010789456973</v>
       </c>
       <c r="F72">
@@ -3181,7 +2832,7 @@
       <c r="D73">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E73" s="4">
+      <c r="E73" s="3">
         <v>4.7300391680339606</v>
       </c>
       <c r="F73">
@@ -3213,7 +2864,7 @@
       <c r="D74">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E74" s="4">
+      <c r="E74" s="3">
         <v>4.6001576441645469</v>
       </c>
       <c r="F74">
@@ -3245,7 +2896,7 @@
       <c r="D75">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E75" s="4">
+      <c r="E75" s="3">
         <v>4.5315236458197932</v>
       </c>
       <c r="F75">
@@ -3277,7 +2928,7 @@
       <c r="D76">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E76" s="4">
+      <c r="E76" s="3">
         <v>4.6170987568533652</v>
       </c>
       <c r="F76">
@@ -3309,7 +2960,7 @@
       <c r="D77">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E77" s="4">
+      <c r="E77" s="3">
         <v>4.5859873665713176</v>
       </c>
       <c r="F77">
@@ -3341,7 +2992,7 @@
       <c r="D78">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E78" s="4">
+      <c r="E78" s="3">
         <v>4.6366688530474622</v>
       </c>
       <c r="F78">
@@ -3373,7 +3024,7 @@
       <c r="D79">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E79" s="4">
+      <c r="E79" s="3">
         <v>4.6549122778829055</v>
       </c>
       <c r="F79">
@@ -3405,7 +3056,7 @@
       <c r="D80">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E80" s="4">
+      <c r="E80" s="3">
         <v>4.6111522576656387</v>
       </c>
       <c r="F80">
@@ -3437,7 +3088,7 @@
       <c r="D81">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E81" s="4">
+      <c r="E81" s="3">
         <v>4.623010104116422</v>
       </c>
       <c r="F81">
@@ -3469,7 +3120,7 @@
       <c r="D82">
         <v>-2.2778924804036742</v>
       </c>
-      <c r="E82" s="4">
+      <c r="E82" s="3">
         <v>4.6520537718869415</v>
       </c>
       <c r="F82">
@@ -3501,7 +3152,7 @@
       <c r="D83">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E83" s="4">
+      <c r="E83" s="3">
         <v>4.8146204101702983</v>
       </c>
       <c r="F83">
@@ -3533,7 +3184,7 @@
       <c r="D84">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E84" s="4">
+      <c r="E84" s="3">
         <v>4.7570325352973377</v>
       </c>
       <c r="F84">
@@ -3565,7 +3216,7 @@
       <c r="D85">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E85" s="4">
+      <c r="E85" s="3">
         <v>4.7077267743131834</v>
       </c>
       <c r="F85">
@@ -3597,7 +3248,7 @@
       <c r="D86">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E86" s="4">
+      <c r="E86" s="3">
         <v>4.580877493419047</v>
       </c>
       <c r="F86">
@@ -3629,7 +3280,7 @@
       <c r="D87">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E87" s="4">
+      <c r="E87" s="3">
         <v>4.5443580465913342</v>
       </c>
       <c r="F87">
@@ -3661,7 +3312,7 @@
       <c r="D88">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E88" s="4">
+      <c r="E88" s="3">
         <v>4.6709579265260945</v>
       </c>
       <c r="F88">
@@ -3693,7 +3344,7 @@
       <c r="D89">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E89" s="4">
+      <c r="E89" s="3">
         <v>4.6337576428400036</v>
       </c>
       <c r="F89">
@@ -3725,7 +3376,7 @@
       <c r="D90">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E90" s="4">
+      <c r="E90" s="3">
         <v>4.7041101338429954</v>
       </c>
       <c r="F90">
@@ -3757,7 +3408,7 @@
       <c r="D91">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E91" s="4">
+      <c r="E91" s="3">
         <v>4.6858280890055459</v>
       </c>
       <c r="F91">
@@ -3789,7 +3440,7 @@
       <c r="D92">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E92" s="4">
+      <c r="E92" s="3">
         <v>4.6812048722640887</v>
       </c>
       <c r="F92">
@@ -3821,7 +3472,7 @@
       <c r="D93">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E93" s="4">
+      <c r="E93" s="3">
         <v>4.6849051540069446</v>
       </c>
       <c r="F93">
@@ -3853,7 +3504,7 @@
       <c r="D94">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E94" s="4">
+      <c r="E94" s="3">
         <v>4.7423200241353252</v>
       </c>
       <c r="F94">
@@ -3885,7 +3536,7 @@
       <c r="D95">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E95" s="4">
+      <c r="E95" s="3">
         <v>4.8535915444865694</v>
       </c>
       <c r="F95">
@@ -3917,7 +3568,7 @@
       <c r="D96">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E96" s="4">
+      <c r="E96" s="3">
         <v>4.8170505450235908</v>
       </c>
       <c r="F96">
@@ -3949,7 +3600,7 @@
       <c r="D97">
         <v>-1.9310215365615626</v>
       </c>
-      <c r="E97" s="4">
+      <c r="E97" s="3">
         <v>4.7706846244656651</v>
       </c>
       <c r="F97">
@@ -3981,7 +3632,7 @@
       <c r="D98">
         <v>-1.8244892938509738</v>
       </c>
-      <c r="E98" s="4">
+      <c r="E98" s="3">
         <v>4.6415021152354816</v>
       </c>
       <c r="F98">
@@ -4013,7 +3664,7 @@
       <c r="D99">
         <v>-1.8244892938509738</v>
       </c>
-      <c r="E99" s="4">
+      <c r="E99" s="3">
         <v>4.6101577274991303</v>
       </c>
       <c r="F99">
@@ -4045,7 +3696,7 @@
       <c r="D100">
         <v>-1.8244892938509738</v>
       </c>
-      <c r="E100" s="4">
+      <c r="E100" s="3">
         <v>4.7032039262594569</v>
       </c>
       <c r="F100">
@@ -4077,7 +3728,7 @@
       <c r="D101">
         <v>-1.8244892938509738</v>
       </c>
-      <c r="E101" s="4">
+      <c r="E101" s="3">
         <v>4.677490847567717</v>
       </c>
       <c r="F101">
@@ -4109,7 +3760,7 @@
       <c r="D102">
         <v>-1.8244892938509738</v>
       </c>
-      <c r="E102" s="4">
+      <c r="E102" s="3">
         <v>4.715816706075155</v>
       </c>
       <c r="F102">
@@ -4141,7 +3792,7 @@
       <c r="D103">
         <v>-1.8244892938509738</v>
       </c>
-      <c r="E103" s="4">
+      <c r="E103" s="3">
         <v>4.7431914838854663</v>
       </c>
       <c r="F103">
@@ -4173,7 +3824,7 @@
       <c r="D104">
         <v>-1.8244892938509738</v>
       </c>
-      <c r="E104" s="4">
+      <c r="E104" s="3">
         <v>4.7167115607209986</v>
       </c>
       <c r="F104">
@@ -4205,7 +3856,7 @@
       <c r="D105">
         <v>-1.8244892938509738</v>
       </c>
-      <c r="E105" s="4">
+      <c r="E105" s="3">
         <v>4.6812048722640887</v>
       </c>
       <c r="F105">
@@ -4237,7 +3888,7 @@
       <c r="D106">
         <v>-1.8244892938509738</v>
       </c>
-      <c r="E106" s="4">
+      <c r="E106" s="3">
         <v>4.7841528415165318</v>
       </c>
       <c r="F106">
@@ -4269,7 +3920,7 @@
       <c r="D107">
         <v>-1.8244892938509738</v>
       </c>
-      <c r="E107" s="4">
+      <c r="E107" s="3">
         <v>4.8473317431380627</v>
       </c>
       <c r="F107">
@@ -4301,7 +3952,7 @@
       <c r="D108">
         <v>-1.8244892938509738</v>
       </c>
-      <c r="E108" s="4">
+      <c r="E108" s="3">
         <v>4.8489003709106893</v>
       </c>
       <c r="F108">
@@ -4333,7 +3984,7 @@
       <c r="D109">
         <v>-1.8244892938509738</v>
       </c>
-      <c r="E109" s="4">
+      <c r="E109" s="3">
         <v>4.8194747886350964</v>
       </c>
       <c r="F109">
@@ -4365,7 +4016,7 @@
       <c r="D110">
         <v>-1.6739764335716716</v>
       </c>
-      <c r="E110" s="4">
+      <c r="E110" s="3">
         <v>4.7184988712950942</v>
       </c>
       <c r="F110">
@@ -4397,7 +4048,7 @@
       <c r="D111">
         <v>-1.6739764335716716</v>
       </c>
-      <c r="E111" s="4">
+      <c r="E111" s="3">
         <v>4.6453519756209234</v>
       </c>
       <c r="F111">
@@ -4429,7 +4080,7 @@
       <c r="D112">
         <v>-1.6739764335716716</v>
       </c>
-      <c r="E112" s="4">
+      <c r="E112" s="3">
         <v>4.7449321283632502</v>
       </c>
       <c r="F112">
@@ -4461,7 +4112,7 @@
       <c r="D113">
         <v>-1.6739764335716716</v>
       </c>
-      <c r="E113" s="4">
+      <c r="E113" s="3">
         <v>4.7184988712950942</v>
       </c>
       <c r="F113">
@@ -4493,7 +4144,7 @@
       <c r="D114">
         <v>-1.6739764335716716</v>
       </c>
-      <c r="E114" s="4">
+      <c r="E114" s="3">
         <v>4.7405748229942946</v>
       </c>
       <c r="F114">
@@ -4525,7 +4176,7 @@
       <c r="D115">
         <v>-1.6739764335716716</v>
       </c>
-      <c r="E115" s="4">
+      <c r="E115" s="3">
         <v>4.7587492739163917</v>
       </c>
       <c r="F115">
@@ -4557,7 +4208,7 @@
       <c r="D116">
         <v>-1.6739764335716716</v>
       </c>
-      <c r="E116" s="4">
+      <c r="E116" s="3">
         <v>4.7621739347977563</v>
       </c>
       <c r="F116">
@@ -4589,7 +4240,7 @@
       <c r="D117">
         <v>-1.6739764335716716</v>
       </c>
-      <c r="E117" s="4">
+      <c r="E117" s="3">
         <v>4.7167115607209986</v>
       </c>
       <c r="F117">
@@ -4621,7 +4272,7 @@
       <c r="D118">
         <v>-1.6739764335716716</v>
       </c>
-      <c r="E118" s="4">
+      <c r="E118" s="3">
         <v>4.808111029984782</v>
       </c>
       <c r="F118">
@@ -4653,7 +4304,7 @@
       <c r="D119">
         <v>-1.6739764335716716</v>
       </c>
-      <c r="E119" s="4">
+      <c r="E119" s="3">
         <v>4.8895969657191998</v>
       </c>
       <c r="F119">
@@ -4685,7 +4336,7 @@
       <c r="D120">
         <v>-1.6739764335716716</v>
       </c>
-      <c r="E120" s="4">
+      <c r="E120" s="3">
         <v>4.8865826454262766</v>
       </c>
       <c r="F120">
@@ -4717,7 +4368,7 @@
       <c r="D121">
         <v>-1.6739764335716716</v>
       </c>
-      <c r="E121" s="4">
+      <c r="E121" s="3">
         <v>4.8528112089026889</v>
       </c>
       <c r="F121">
@@ -4749,7 +4400,7 @@
       <c r="D122">
         <v>-1.6739764335716716</v>
       </c>
-      <c r="E122" s="4">
+      <c r="E122" s="3">
         <v>4.6959245492565556</v>
       </c>
       <c r="F122">
@@ -4781,7 +4432,7 @@
       <c r="D123">
         <v>-1.6739764335716716</v>
       </c>
-      <c r="E123" s="4">
+      <c r="E123" s="3">
         <v>4.6709579265260945</v>
       </c>
       <c r="F123">
@@ -4804,1371 +4455,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J41"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="3">
-        <v>22.85080676806621</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.61070239666055792</v>
-      </c>
-      <c r="D2" s="3">
-        <v>-4.6051701859880909</v>
-      </c>
-      <c r="E2">
-        <f>LN([1]Sheet2!H2)</f>
-        <v>16.808603501549189</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="3">
-        <v>22.972427196617996</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.60808873862853263</v>
-      </c>
-      <c r="D3" s="3">
-        <v>-4.6051701859880909</v>
-      </c>
-      <c r="E3">
-        <f>LN([1]Sheet2!H3)</f>
-        <v>16.887164582779718</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3">
-        <v>22.993171253569333</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.70976130483683475</v>
-      </c>
-      <c r="D4" s="3">
-        <v>-3.4106638731693883</v>
-      </c>
-      <c r="E4">
-        <f>LN([1]Sheet2!H4)</f>
-        <v>17.047246140562017</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3">
-        <v>22.794296528515947</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.75974558663000746</v>
-      </c>
-      <c r="D5" s="3">
-        <v>-2.8134107167600368</v>
-      </c>
-      <c r="E5">
-        <f>LN([1]Sheet2!H5)</f>
-        <v>16.978929273893449</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="3">
-        <v>22.783989104543185</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.82765737228041003</v>
-      </c>
-      <c r="D6" s="3">
-        <v>-2.8134107167600368</v>
-      </c>
-      <c r="E6">
-        <f>LN([1]Sheet2!H6)</f>
-        <v>16.866360127582766</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="3">
-        <v>22.967594531881947</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.7930739635125913</v>
-      </c>
-      <c r="D7" s="3">
-        <v>-2.8134107167600368</v>
-      </c>
-      <c r="E7">
-        <f>LN([1]Sheet2!H7)</f>
-        <v>16.980064844781985</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="3">
-        <v>22.98445713691854</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.7793730176631205</v>
-      </c>
-      <c r="D8" s="3">
-        <v>-2.8134107167600368</v>
-      </c>
-      <c r="E8">
-        <f>LN([1]Sheet2!H8)</f>
-        <v>17.108245952708334</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="3">
-        <v>22.91553670620679</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.75294478378154783</v>
-      </c>
-      <c r="D9" s="3">
-        <v>-2.8134107167600368</v>
-      </c>
-      <c r="E9">
-        <f>LN([1]Sheet2!H9)</f>
-        <v>17.0348043354781</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="3">
-        <v>22.797078668374397</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.76743611948518786</v>
-      </c>
-      <c r="D10" s="3">
-        <v>-2.7106435968751974</v>
-      </c>
-      <c r="E10">
-        <f>LN([1]Sheet2!H10)</f>
-        <v>16.944207813762709</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="3">
-        <v>22.913826478733238</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.80583003434131195</v>
-      </c>
-      <c r="D11" s="3">
-        <v>-2.6592600369327779</v>
-      </c>
-      <c r="E11">
-        <f>LN([1]Sheet2!H11)</f>
-        <v>17.017485483847636</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="3">
-        <v>22.971872202135074</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0.80730132508388819</v>
-      </c>
-      <c r="D12" s="3">
-        <v>-2.6592600369327779</v>
-      </c>
-      <c r="E12">
-        <f>LN([1]Sheet2!H12)</f>
-        <v>17.139544890087979</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="3">
-        <v>22.935464303969951</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.80655213684516591</v>
-      </c>
-      <c r="D13" s="3">
-        <v>-2.6132647892748104</v>
-      </c>
-      <c r="E13">
-        <f>LN([1]Sheet2!H13)</f>
-        <v>17.075805830841844</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="3">
-        <v>22.81583625079486</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.82337354085813186</v>
-      </c>
-      <c r="D14" s="3">
-        <v>-2.5902671654458267</v>
-      </c>
-      <c r="E14">
-        <f>LN([1]Sheet2!H14)</f>
-        <v>17.011957239661367</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="3">
-        <v>22.948125593713328</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0.78664339636442049</v>
-      </c>
-      <c r="D15" s="3">
-        <v>-2.5902671654458267</v>
-      </c>
-      <c r="E15">
-        <f>LN([1]Sheet2!H15)</f>
-        <v>17.043400632133626</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="3">
-        <v>22.973205411544924</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0.78698041467219315</v>
-      </c>
-      <c r="D16" s="3">
-        <v>-2.5902671654458267</v>
-      </c>
-      <c r="E16">
-        <f>LN([1]Sheet2!H16)</f>
-        <v>17.148061151103004</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="3">
-        <v>22.92517114611849</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0.75651935114073543</v>
-      </c>
-      <c r="D17" s="3">
-        <v>-2.5902671654458267</v>
-      </c>
-      <c r="E17">
-        <f>LN([1]Sheet2!H17)</f>
-        <v>17.003520907265052</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="3">
-        <v>22.864429816296802</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0.75571649576223798</v>
-      </c>
-      <c r="D18" s="3">
-        <v>-2.5902671654458267</v>
-      </c>
-      <c r="E18">
-        <f>LN([1]Sheet2!H18)</f>
-        <v>16.852518739004442</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="3">
-        <v>23.003870030667787</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0.79797012429722136</v>
-      </c>
-      <c r="D19" s="3">
-        <v>-2.4861422704317757</v>
-      </c>
-      <c r="E19">
-        <f>LN([1]Sheet2!H19)</f>
-        <v>16.962556533784671</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="3">
-        <v>22.867745099748252</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0.90733167922011904</v>
-      </c>
-      <c r="D20" s="3">
-        <v>-2.2778924804036742</v>
-      </c>
-      <c r="E20">
-        <f>LN([1]Sheet2!H20)</f>
-        <v>17.119942234392049</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="3">
-        <v>22.909878017859544</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0.87834654205988982</v>
-      </c>
-      <c r="D21" s="3">
-        <v>-2.2778924804036742</v>
-      </c>
-      <c r="E21">
-        <f>LN([1]Sheet2!H21)</f>
-        <v>17.060445125257036</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="3">
-        <v>22.636614733814799</v>
-      </c>
-      <c r="C22" s="3">
-        <v>1.05781183915413</v>
-      </c>
-      <c r="D22" s="3">
-        <v>-2.2778924804036742</v>
-      </c>
-      <c r="E22">
-        <f>LN([1]Sheet2!H22)</f>
-        <v>16.971119799106109</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="3">
-        <v>22.830679561952607</v>
-      </c>
-      <c r="C23" s="3">
-        <v>1.0634751214773148</v>
-      </c>
-      <c r="D23" s="3">
-        <v>-2.2778924804036742</v>
-      </c>
-      <c r="E23">
-        <f>LN([1]Sheet2!H23)</f>
-        <v>17.061700025812417</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="3">
-        <v>22.809278822234045</v>
-      </c>
-      <c r="C24" s="3">
-        <v>1.0753572532848905</v>
-      </c>
-      <c r="D24" s="3">
-        <v>-2.2778924804036742</v>
-      </c>
-      <c r="E24">
-        <f>LN([1]Sheet2!H24)</f>
-        <v>17.171348339338032</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="3">
-        <v>22.801705439206319</v>
-      </c>
-      <c r="C25" s="3">
-        <v>1.0419905848227948</v>
-      </c>
-      <c r="D25" s="3">
-        <v>-2.2778924804036742</v>
-      </c>
-      <c r="E25">
-        <f>LN([1]Sheet2!H25)</f>
-        <v>17.149729110023394</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="3">
-        <v>22.617217853993921</v>
-      </c>
-      <c r="C26" s="3">
-        <v>1.0362248851491658</v>
-      </c>
-      <c r="D26" s="3">
-        <v>-2.2778924804036742</v>
-      </c>
-      <c r="E26">
-        <f>LN([1]Sheet2!H26)</f>
-        <v>17.088223484995801</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="3">
-        <v>22.806533954828936</v>
-      </c>
-      <c r="C27" s="3">
-        <v>1.0171245969415954</v>
-      </c>
-      <c r="D27" s="3">
-        <v>-2.2778924804036742</v>
-      </c>
-      <c r="E27">
-        <f>LN([1]Sheet2!H27)</f>
-        <v>17.150657520591452</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="3">
-        <v>22.864506049827767</v>
-      </c>
-      <c r="C28" s="3">
-        <v>1.0214134435303384</v>
-      </c>
-      <c r="D28" s="3">
-        <v>-2.2778924804036742</v>
-      </c>
-      <c r="E28">
-        <f>LN([1]Sheet2!H28)</f>
-        <v>17.255181161939568</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="3">
-        <v>22.689035084884807</v>
-      </c>
-      <c r="C29" s="3">
-        <v>1.101459165659991</v>
-      </c>
-      <c r="D29" s="3">
-        <v>-1.9310215365615626</v>
-      </c>
-      <c r="E29">
-        <f>LN([1]Sheet2!H29)</f>
-        <v>17.201009020589655</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="3">
-        <v>22.649583455055847</v>
-      </c>
-      <c r="C30" s="3">
-        <v>1.1075487304746343</v>
-      </c>
-      <c r="D30" s="3">
-        <v>-1.9310215365615626</v>
-      </c>
-      <c r="E30">
-        <f>LN([1]Sheet2!H30)</f>
-        <v>17.118610943587793</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="3">
-        <v>22.867293343680895</v>
-      </c>
-      <c r="C31" s="3">
-        <v>1.0929105886399468</v>
-      </c>
-      <c r="D31" s="3">
-        <v>-1.9310215365615626</v>
-      </c>
-      <c r="E31">
-        <f>LN([1]Sheet2!H31)</f>
-        <v>17.177782132317478</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="3">
-        <v>22.889199071806825</v>
-      </c>
-      <c r="C32" s="3">
-        <v>1.1018030320686176</v>
-      </c>
-      <c r="D32" s="3">
-        <v>-1.9310215365615626</v>
-      </c>
-      <c r="E32">
-        <f>LN([1]Sheet2!H32)</f>
-        <v>17.270045083929045</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="3">
-        <v>22.909611225921825</v>
-      </c>
-      <c r="C33" s="3">
-        <v>1.0651126460529936</v>
-      </c>
-      <c r="D33" s="3">
-        <v>-1.9310215365615626</v>
-      </c>
-      <c r="E33">
-        <f>LN([1]Sheet2!H33)</f>
-        <v>17.214371011134887</v>
-      </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="3">
-        <v>22.542360886900422</v>
-      </c>
-      <c r="C34" s="3">
-        <v>1.1757658461141931</v>
-      </c>
-      <c r="D34" s="3">
-        <v>-1.8244892938509738</v>
-      </c>
-      <c r="E34">
-        <f>LN([1]Sheet2!H34)</f>
-        <v>17.149424106900415</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-      <c r="I34">
-        <v>1</v>
-      </c>
-      <c r="J34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="3">
-        <v>22.765906651003771</v>
-      </c>
-      <c r="C35" s="3">
-        <v>1.1818085603840507</v>
-      </c>
-      <c r="D35" s="3">
-        <v>-1.8244892938509738</v>
-      </c>
-      <c r="E35">
-        <f>LN([1]Sheet2!H35)</f>
-        <v>17.223509754745358</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-      <c r="J35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" s="3">
-        <v>22.824371568493202</v>
-      </c>
-      <c r="C36" s="3">
-        <v>1.1759731317298414</v>
-      </c>
-      <c r="D36" s="3">
-        <v>-1.8244892938509738</v>
-      </c>
-      <c r="E36">
-        <f>LN([1]Sheet2!H36)</f>
-        <v>17.312186256810026</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36">
-        <v>1</v>
-      </c>
-      <c r="J36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="3">
-        <v>22.851937060218219</v>
-      </c>
-      <c r="C37" s="3">
-        <v>1.1245030035455026</v>
-      </c>
-      <c r="D37" s="3">
-        <v>-1.8244892938509738</v>
-      </c>
-      <c r="E37">
-        <f>LN([1]Sheet2!H37)</f>
-        <v>17.259073318516059</v>
-      </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
-      <c r="I37">
-        <v>1</v>
-      </c>
-      <c r="J37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" s="3">
-        <v>22.522698693564923</v>
-      </c>
-      <c r="C38" s="3">
-        <v>1.1166335485310592</v>
-      </c>
-      <c r="D38" s="3">
-        <v>-1.6739764335716716</v>
-      </c>
-      <c r="E38">
-        <f>LN([1]Sheet2!H38)</f>
-        <v>17.196939049761138</v>
-      </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-      <c r="I38">
-        <v>1</v>
-      </c>
-      <c r="J38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B39" s="3">
-        <v>22.803189990046132</v>
-      </c>
-      <c r="C39" s="3">
-        <v>1.1045366295570438</v>
-      </c>
-      <c r="D39" s="3">
-        <v>-1.6739764335716716</v>
-      </c>
-      <c r="E39">
-        <f>LN([1]Sheet2!H39)</f>
-        <v>17.24650684249135</v>
-      </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-      <c r="I39">
-        <v>1</v>
-      </c>
-      <c r="J39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="3">
-        <v>22.890222366949342</v>
-      </c>
-      <c r="C40" s="3">
-        <v>1.1127208577763688</v>
-      </c>
-      <c r="D40" s="3">
-        <v>-1.6739764335716716</v>
-      </c>
-      <c r="E40">
-        <f>LN([1]Sheet2!H40)</f>
-        <v>17.331387646416584</v>
-      </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-      <c r="I40">
-        <v>1</v>
-      </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41" s="3">
-        <v>22.886136830919813</v>
-      </c>
-      <c r="C41" s="3">
-        <v>1.0839527025381182</v>
-      </c>
-      <c r="D41" s="3">
-        <v>-1.6739764335716716</v>
-      </c>
-      <c r="E41">
-        <f>LN([1]Sheet2!H41)</f>
-        <v>17.284497046879846</v>
-      </c>
-      <c r="F41">
-        <v>1</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="H41">
-        <v>1</v>
-      </c>
-      <c r="I41">
-        <v>1</v>
-      </c>
-      <c r="J41">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>